<commit_message>
reimplement bitonic sort, begin writing final report, compile results, and get modified results from bitonic sort
</commit_message>
<xml_diff>
--- a/results/bucketsort.xlsx
+++ b/results/bucketsort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ValkCoen\Documents\school\parallel_prog\CSCI4320-FinalProject\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{6FFEC1CA-BB52-4192-84B9-50094BE729EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C169C278-9D93-46DF-9445-42302EBFEFEF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E42E4912-2D05-4ADE-A725-3FECD4A733B3}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_Sheet1A1G131" hidden="1">Sheet1!$A$1:$G$13</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Sheet1A1G13" hidden="1">Sheet1!$A$1:$G$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,16 +55,12 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1A1G131"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1A1G13"/>
         </x15:connection>
       </ext>
     </extLst>
   </connection>
 </connections>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -132,6 +128,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Scalability of Bucketsort - 1048576</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Elements</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -170,6 +196,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -287,7 +324,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D3DF-4AC9-96B9-186A25909E58}"/>
+              <c16:uniqueId val="{00000000-804E-4E78-920A-1F4177CC9B01}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -299,11 +336,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1566593055"/>
-        <c:axId val="583773119"/>
+        <c:axId val="728451264"/>
+        <c:axId val="764170384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1566593055"/>
+        <c:axId val="728451264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -323,6 +360,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Processes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -360,12 +456,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="583773119"/>
+        <c:crossAx val="764170384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="583773119"/>
+        <c:axId val="764170384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -385,6 +481,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -422,7 +578,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1566593055"/>
+        <c:crossAx val="728451264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -436,6 +592,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -486,6 +649,39 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Execution Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Bucketsort - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>512 Ranks</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -519,18 +715,18 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2097152</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -561,95 +757,62 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1048576</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2097152</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>4194304</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>8388608</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32</c:v>
+                  <c:v>16777216</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4096</c:v>
+                  <c:v>33554432</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$13</c:f>
+              <c:f>Sheet1!$B$10:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>223.40918400000001</c:v>
+                  <c:v>7.1632309999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.267991000000002</c:v>
+                  <c:v>14.334215</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.322952000000001</c:v>
+                  <c:v>28.645219000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.888826999999999</c:v>
+                  <c:v>57.220145000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.832681999999998</c:v>
+                  <c:v>114.469634</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.755237999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16.766037000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14.354995000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14.334215</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11.300703</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13.935181</c:v>
+                  <c:v>228.85732999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7086-40B6-86F4-DF6BEC54F0AA}"/>
+              <c16:uniqueId val="{00000000-3C64-4030-BB4D-1569823C61AD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -661,11 +824,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="581534271"/>
-        <c:axId val="583785599"/>
+        <c:axId val="165271312"/>
+        <c:axId val="275409888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="581534271"/>
+        <c:axId val="165271312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,6 +848,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Processors</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -722,12 +945,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="583785599"/>
+        <c:crossAx val="275409888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="583785599"/>
+        <c:axId val="275409888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,6 +970,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -784,7 +1067,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="581534271"/>
+        <c:crossAx val="165271312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1956,23 +2239,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37CD0507-E5D3-418F-9D24-7F35D2E32BD6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC2C8707-200F-45BB-805B-A39DFB87591D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1992,23 +2275,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76FD2AEB-0B0D-4D2F-B4DA-08BC7BC2D901}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF1AF61B-D39B-409A-AE09-EFE08083B06F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2329,7 +2612,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A10" activeCellId="1" sqref="A1:XFD1 A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,18 +2627,23 @@
         <v>1048576</v>
       </c>
       <c r="C1">
+        <f>B1 * 2</f>
         <v>2097152</v>
       </c>
       <c r="D1">
-        <v>419304</v>
+        <f t="shared" ref="D1:G1" si="0">C1 * 2</f>
+        <v>4194304</v>
       </c>
       <c r="E1">
+        <f t="shared" si="0"/>
         <v>8388608</v>
       </c>
       <c r="F1">
+        <f t="shared" si="0"/>
         <v>16777216</v>
       </c>
       <c r="G1">
+        <f t="shared" si="0"/>
         <v>33554432</v>
       </c>
     </row>

</xml_diff>